<commit_message>
XLSX: Planilla Parte 1
</commit_message>
<xml_diff>
--- a/planilla.xlsx
+++ b/planilla.xlsx
@@ -13,25 +13,65 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Tony</t>
-  </si>
-  <si>
-    <t>Smithyman</t>
-  </si>
-  <si>
-    <t>Sofie</t>
-  </si>
-  <si>
-    <t>Brett</t>
+    <r>
+      <rPr>
+        <b/>
+        <color theme="1"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+        <sz val="20"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>PLANILLA PRIMER TRIMESTRE (PARTE 1)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">UNIDAD EDUCATIVA: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">ÁREA: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">AÑO DE ESCOLARIDAD: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">MATERIA: </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">MAESTRO (A): </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">GESTIÓN: </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -55,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,12 +103,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -84,6 +137,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127999</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="600075" cy="714375"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -408,55 +505,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor rgb="FFC0000"/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0"/>
-  </sheetViews>
+  <dimension ref="A2:J11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="3" width="20" customWidth="1"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:C1"/>
+  <mergeCells count="1">
+    <mergeCell ref="C2:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <headerFooter>
+    <firstHeader>Hello Exceljs</firstHeader>
+    <firstFooter>Hello World</firstFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>